<commit_message>
Updated CosineSimilarity benchmarks and updated results.
</commit_message>
<xml_diff>
--- a/TextClustering.Benchmark/Results/BenchmarkResults.xlsx
+++ b/TextClustering.Benchmark/Results/BenchmarkResults.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\repo\TextClustering\TextClustering.Benchmark\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{259FDC41-CC04-47EC-A13F-E7163D71A909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52462E81-7E05-4204-8DE5-56C9E681925B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38595" yWindow="900" windowWidth="38010" windowHeight="19785" xr2:uid="{16676089-231D-450F-981F-EF3A68C105B7}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="38610" windowHeight="21705" activeTab="2" xr2:uid="{16676089-231D-450F-981F-EF3A68C105B7}"/>
   </bookViews>
   <sheets>
     <sheet name="CosineSimilarity" sheetId="1" r:id="rId1"/>
     <sheet name="CountVectorizer" sheetId="2" r:id="rId2"/>
+    <sheet name="CosineSimilarityNET8_VS_NET9" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="52">
   <si>
     <t>VectorSize</t>
   </si>
@@ -103,11 +104,116 @@
   <si>
     <t>BERT(dim=384)</t>
   </si>
+  <si>
+    <t>CompulteCosineSimilarityOnFloatArray</t>
+  </si>
+  <si>
+    <t>CompulteCosineSimilarityOnVectors</t>
+  </si>
+  <si>
+    <t>ComputeCosineSimilarityOnNdarray</t>
+  </si>
+  <si>
+    <t>ComputeCosineSimilarityOnDictionary</t>
+  </si>
+  <si>
+    <t>ComputeCosineSimilarityOnDictionaryWithVector</t>
+  </si>
+  <si>
+    <t>ComputeCosineSimilarityOnVector2</t>
+  </si>
+  <si>
+    <t>ComputeCosineSimilarityOnVector3</t>
+  </si>
+  <si>
+    <t>Error (ms)</t>
+  </si>
+  <si>
+    <t>Mean (us)</t>
+  </si>
+  <si>
+    <t>Error (us)</t>
+  </si>
+  <si>
+    <t>4,362.4</t>
+  </si>
+  <si>
+    <t>5,218.5</t>
+  </si>
+  <si>
+    <t>430,476.0</t>
+  </si>
+  <si>
+    <t>126,358.1</t>
+  </si>
+  <si>
+    <t>100,927.1</t>
+  </si>
+  <si>
+    <t>842.9</t>
+  </si>
+  <si>
+    <t>344.7</t>
+  </si>
+  <si>
+    <t>86.75</t>
+  </si>
+  <si>
+    <t>96.17</t>
+  </si>
+  <si>
+    <t>8,605.30</t>
+  </si>
+  <si>
+    <t>1,559.21</t>
+  </si>
+  <si>
+    <t>1,350.54</t>
+  </si>
+  <si>
+    <t>2.96</t>
+  </si>
+  <si>
+    <t>3.20</t>
+  </si>
+  <si>
+    <t>CompulteCosineSimilarityOnFloatArray_NET8</t>
+  </si>
+  <si>
+    <t>ComputeCosineSimilarityOnDictionary_NET8</t>
+  </si>
+  <si>
+    <t>ComputeCosineSimilarityOnNdarray_NET8</t>
+  </si>
+  <si>
+    <t>ComputeCosineSimilarityOnVector2_NET8</t>
+  </si>
+  <si>
+    <t>ComputeCosineSimilarityOnVector3_NET8</t>
+  </si>
+  <si>
+    <t>CompulteCosineSimilarityOnVectors_NET8</t>
+  </si>
+  <si>
+    <t>ComputeCosineSimilarityOnDictionaryWithVector_NET8</t>
+  </si>
+  <si>
+    <t>(NET 9) Mean (ms)</t>
+  </si>
+  <si>
+    <t>(NET 8) Mean (ms)</t>
+  </si>
+  <si>
+    <t>Reduction</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -137,9 +243,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,7 +580,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1265,6 +1372,1518 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sv-SE"/>
+              <a:t>NET</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="sv-SE" baseline="0"/>
+              <a:t> 8 Vs NET 9 - Logarithmic mean (ms)</a:t>
+            </a:r>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sv-SE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>(NET 9) Mean (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$A$20:$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>CompulteCosineSimilarityOnFloatArray</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CompulteCosineSimilarityOnVectors</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ComputeCosineSimilarityOnNdarray</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ComputeCosineSimilarityOnDictionary</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ComputeCosineSimilarityOnDictionaryWithVector</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ComputeCosineSimilarityOnVector2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ComputeCosineSimilarityOnVector3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$B$20:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.62280442780503209</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71252343487769476</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5991000910235207</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0806153047770688</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9965449434408036</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-8.7087448823903096E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.46029676105217449</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-606B-44DC-B5E4-2B3F75F9C4D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$C$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>(NET 8) Mean (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$A$20:$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>CompulteCosineSimilarityOnFloatArray</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CompulteCosineSimilarityOnVectors</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ComputeCosineSimilarityOnNdarray</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ComputeCosineSimilarityOnDictionary</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ComputeCosineSimilarityOnDictionaryWithVector</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ComputeCosineSimilarityOnVector2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ComputeCosineSimilarityOnVector3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$C$20:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.63972548467876489</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71754568780327022</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6339489435757018</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.101603086956763</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0040077945839494</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-7.4223946163253715E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.46255871659205239</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-606B-44DC-B5E4-2B3F75F9C4D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1181451871"/>
+        <c:axId val="1181452351"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1181451871"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1181452351"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1181452351"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1181451871"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sv-SE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sv-SE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sv-SE"/>
+              <a:t>NET 9 vs NET 8 - Time reduction (%)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sv-SE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CompulteCosineSimilarityOnFloatArray</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="sv-SE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$G$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Reduction</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$G$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.8212910324592064E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0346-43E5-B846-0F367F7A5944}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CompulteCosineSimilarityOnVectors</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="sv-SE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$G$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Reduction</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.1497556769186512E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0346-43E5-B846-0F367F7A5944}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ComputeCosineSimilarityOnNdarray</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="sv-SE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$G$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Reduction</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7.7107434560811816E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0346-43E5-B846-0F367F7A5944}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ComputeCosineSimilarityOnDictionary</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="sv-SE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$G$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Reduction</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4.7177030993660218E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0346-43E5-B846-0F367F7A5944}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ComputeCosineSimilarityOnDictionaryWithVector</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="sv-SE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$G$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Reduction</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$G$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.7037049513956237E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-0346-43E5-B846-0F367F7A5944}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ComputeCosineSimilarityOnVector2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="sv-SE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$G$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Reduction</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$G$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2.9184956697117181E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-0346-43E5-B846-0F367F7A5944}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ComputeCosineSimilarityOnVector3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="sv-SE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$G$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Reduction</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CosineSimilarityNET8_VS_NET9!$G$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-5.2219321148823106E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-0346-43E5-B846-0F367F7A5944}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="926362015"/>
+        <c:axId val="1180688319"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="926362015"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1180688319"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1180688319"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="926362015"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sv-SE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sv-SE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
@@ -1339,6 +2958,83 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2313,6 +4009,1016 @@
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2419,6 +5125,83 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>576261</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>371474</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92588AA7-56B2-60ED-9054-A14E3AEBD0FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>581026</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>77528</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>466726</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4653A529-C8D3-96FC-DA12-3C74268C46B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2746,7 +5529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A384F70-555A-4521-98DD-F85E42E001B4}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
@@ -3380,11 +6163,11 @@
         <v>100</v>
       </c>
       <c r="C8">
-        <f>LOG(E8)</f>
+        <f t="shared" ref="C8:D11" si="3">LOG(E8)</f>
         <v>0.11925588927793671</v>
       </c>
       <c r="D8">
-        <f>LOG(F8)</f>
+        <f t="shared" si="3"/>
         <v>-2.5228787452803374</v>
       </c>
       <c r="E8">
@@ -3402,11 +6185,11 @@
         <v>100</v>
       </c>
       <c r="C9">
-        <f>LOG(E9)</f>
+        <f t="shared" si="3"/>
         <v>-0.22865067478182449</v>
       </c>
       <c r="D9">
-        <f>LOG(F9)</f>
+        <f t="shared" si="3"/>
         <v>-2.5523769022397138</v>
       </c>
       <c r="E9">
@@ -3424,11 +6207,11 @@
         <v>100</v>
       </c>
       <c r="C10">
-        <f>LOG(E10)</f>
+        <f t="shared" si="3"/>
         <v>-0.16322662828193052</v>
       </c>
       <c r="D10">
-        <f>LOG(F10)</f>
+        <f t="shared" si="3"/>
         <v>-2.6603498423863159</v>
       </c>
       <c r="E10">
@@ -3446,11 +6229,11 @@
         <v>100</v>
       </c>
       <c r="C11">
-        <f>LOG(E11)</f>
+        <f t="shared" si="3"/>
         <v>-0.32999734567858685</v>
       </c>
       <c r="D11">
-        <f>LOG(F11)</f>
+        <f t="shared" si="3"/>
         <v>-2.6963720236161102</v>
       </c>
       <c r="E11">
@@ -3468,11 +6251,11 @@
         <v>100</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12" si="3">LOG(E12)</f>
+        <f t="shared" ref="C12" si="4">LOG(E12)</f>
         <v>3.2779757462232233</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12" si="4">LOG(F12)</f>
+        <f t="shared" ref="D12" si="5">LOG(F12)</f>
         <v>1.4571246263034088</v>
       </c>
       <c r="E12">
@@ -3490,11 +6273,11 @@
         <v>1000</v>
       </c>
       <c r="C14">
-        <f>LOG(E14)</f>
+        <f t="shared" ref="C14:D17" si="6">LOG(E14)</f>
         <v>1.1751927883866031</v>
       </c>
       <c r="D14">
-        <f>LOG(F14)</f>
+        <f t="shared" si="6"/>
         <v>-1.4685210829577449</v>
       </c>
       <c r="E14">
@@ -3512,11 +6295,11 @@
         <v>1000</v>
       </c>
       <c r="C15">
-        <f>LOG(E15)</f>
+        <f t="shared" si="6"/>
         <v>0.7606486195813561</v>
       </c>
       <c r="D15">
-        <f>LOG(F15)</f>
+        <f t="shared" si="6"/>
         <v>-1.7695510786217261</v>
       </c>
       <c r="E15">
@@ -3534,11 +6317,11 @@
         <v>1000</v>
       </c>
       <c r="C16">
-        <f>LOG(E16)</f>
+        <f t="shared" si="6"/>
         <v>0.8583567052977733</v>
       </c>
       <c r="D16">
-        <f>LOG(F16)</f>
+        <f t="shared" si="6"/>
         <v>-1.5376020021010439</v>
       </c>
       <c r="E16">
@@ -3556,11 +6339,11 @@
         <v>1000</v>
       </c>
       <c r="C17">
-        <f>LOG(E17)</f>
+        <f t="shared" si="6"/>
         <v>0.77378644498119353</v>
       </c>
       <c r="D17">
-        <f>LOG(F17)</f>
+        <f t="shared" si="6"/>
         <v>-1.744727494896694</v>
       </c>
       <c r="E17">
@@ -3578,11 +6361,11 @@
         <v>1000</v>
       </c>
       <c r="C18">
-        <f t="shared" ref="C18" si="5">LOG(E18)</f>
+        <f t="shared" ref="C18" si="7">LOG(E18)</f>
         <v>4.1990691962517417</v>
       </c>
       <c r="D18">
-        <f t="shared" ref="D18" si="6">LOG(F18)</f>
+        <f t="shared" ref="D18" si="8">LOG(F18)</f>
         <v>2.0232936230366052</v>
       </c>
       <c r="E18">
@@ -3600,11 +6383,11 @@
         <v>10000</v>
       </c>
       <c r="C20">
-        <f>LOG(E20)</f>
+        <f t="shared" ref="C20:D23" si="9">LOG(E20)</f>
         <v>2.3334251057671449</v>
       </c>
       <c r="D20">
-        <f>LOG(F20)</f>
+        <f t="shared" si="9"/>
         <v>1.7450729510536125E-2</v>
       </c>
       <c r="E20">
@@ -3622,11 +6405,11 @@
         <v>10000</v>
       </c>
       <c r="C21">
-        <f>LOG(E21)</f>
+        <f t="shared" si="9"/>
         <v>2.1543143965637754</v>
       </c>
       <c r="D21">
-        <f>LOG(F21)</f>
+        <f t="shared" si="9"/>
         <v>-8.8842391260023412E-2</v>
       </c>
       <c r="E21">
@@ -3644,11 +6427,11 @@
         <v>10000</v>
       </c>
       <c r="C22">
-        <f>LOG(E22)</f>
+        <f t="shared" si="9"/>
         <v>2.2055048004518092</v>
       </c>
       <c r="D22">
-        <f>LOG(F22)</f>
+        <f t="shared" si="9"/>
         <v>-0.10292299679057967</v>
       </c>
       <c r="E22">
@@ -3666,11 +6449,11 @@
         <v>10000</v>
       </c>
       <c r="C23">
-        <f>LOG(E23)</f>
+        <f t="shared" si="9"/>
         <v>2.1393626613992449</v>
       </c>
       <c r="D23">
-        <f>LOG(F23)</f>
+        <f t="shared" si="9"/>
         <v>-0.10513034325474745</v>
       </c>
       <c r="E23">
@@ -3688,11 +6471,11 @@
         <v>100000</v>
       </c>
       <c r="C25">
-        <f>LOG(E25)</f>
+        <f t="shared" ref="C25:D28" si="10">LOG(E25)</f>
         <v>3.4094258686714434</v>
       </c>
       <c r="D25">
-        <f>LOG(F25)</f>
+        <f t="shared" si="10"/>
         <v>1.0413926851582251</v>
       </c>
       <c r="E25">
@@ -3710,11 +6493,11 @@
         <v>100000</v>
       </c>
       <c r="C26">
-        <f>LOG(E26)</f>
+        <f t="shared" si="10"/>
         <v>3.1806992012960347</v>
       </c>
       <c r="D26">
-        <f>LOG(F26)</f>
+        <f t="shared" si="10"/>
         <v>0.90308998699194354</v>
       </c>
       <c r="E26">
@@ -3732,11 +6515,11 @@
         <v>100000</v>
       </c>
       <c r="C27">
-        <f>LOG(E27)</f>
+        <f t="shared" si="10"/>
         <v>3.2968844755385471</v>
       </c>
       <c r="D27">
-        <f>LOG(F27)</f>
+        <f t="shared" si="10"/>
         <v>0.84509804001425681</v>
       </c>
       <c r="E27">
@@ -3754,11 +6537,11 @@
         <v>100000</v>
       </c>
       <c r="C28">
-        <f>LOG(E28)</f>
+        <f t="shared" si="10"/>
         <v>3.1720188094245563</v>
       </c>
       <c r="D28">
-        <f>LOG(F28)</f>
+        <f t="shared" si="10"/>
         <v>0.90308998699194354</v>
       </c>
       <c r="E28">
@@ -3771,6 +6554,543 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749583F7-52D1-4AEF-8FEF-4547B6F57345}">
+  <dimension ref="A1:H26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y9" sqref="Y9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2">
+        <f t="shared" ref="B2:C8" si="0">E2/1000</f>
+        <v>4.1956999999999995</v>
+      </c>
+      <c r="C2" s="2">
+        <f t="shared" si="0"/>
+        <v>8.3430000000000004E-2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>4195.7</v>
+      </c>
+      <c r="F2" s="2">
+        <v>83.43</v>
+      </c>
+      <c r="G2">
+        <v>256</v>
+      </c>
+      <c r="H2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2">
+        <f t="shared" si="0"/>
+        <v>5.1585000000000001</v>
+      </c>
+      <c r="C3" s="2">
+        <f t="shared" si="0"/>
+        <v>0.10217</v>
+      </c>
+      <c r="E3" s="2">
+        <v>5158.5</v>
+      </c>
+      <c r="F3" s="2">
+        <v>102.17</v>
+      </c>
+      <c r="G3">
+        <v>256</v>
+      </c>
+      <c r="H3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2">
+        <f t="shared" si="0"/>
+        <v>397.28309999999999</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" si="0"/>
+        <v>7.9236199999999997</v>
+      </c>
+      <c r="E4" s="2">
+        <v>397283.1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>7923.62</v>
+      </c>
+      <c r="G4">
+        <v>256</v>
+      </c>
+      <c r="H4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2">
+        <f t="shared" si="0"/>
+        <v>120.39689999999999</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.94246000000000008</v>
+      </c>
+      <c r="E5" s="2">
+        <v>120396.9</v>
+      </c>
+      <c r="F5" s="2">
+        <v>942.46</v>
+      </c>
+      <c r="G5">
+        <v>256</v>
+      </c>
+      <c r="H5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2">
+        <f t="shared" si="0"/>
+        <v>99.207599999999999</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0365199999999999</v>
+      </c>
+      <c r="E6" s="2">
+        <v>99207.6</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1036.52</v>
+      </c>
+      <c r="G6">
+        <v>256</v>
+      </c>
+      <c r="H6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.81829999999999992</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="0"/>
+        <v>1.98E-3</v>
+      </c>
+      <c r="E7" s="2">
+        <v>818.3</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="G7">
+        <v>256</v>
+      </c>
+      <c r="H7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.34649999999999997</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>2.5499999999999997E-3</v>
+      </c>
+      <c r="E8" s="2">
+        <v>346.5</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="G8">
+        <v>256</v>
+      </c>
+      <c r="H8">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="2">
+        <f t="shared" ref="B10:C16" si="1">E10/1000</f>
+        <v>4.3624000000000001</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="1"/>
+        <v>8.6749999999999994E-2</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="2">
+        <f t="shared" si="1"/>
+        <v>5.2184999999999997</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="1"/>
+        <v>9.6170000000000005E-2</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="2">
+        <f t="shared" si="1"/>
+        <v>430.476</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="1"/>
+        <v>8.6052999999999997</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="2">
+        <f t="shared" si="1"/>
+        <v>126.35810000000001</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="1"/>
+        <v>1.55921</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="2">
+        <f t="shared" si="1"/>
+        <v>100.92710000000001</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3505400000000001</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="2">
+        <f t="shared" si="1"/>
+        <v>0.84289999999999998</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="1"/>
+        <v>2.96E-3</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="2">
+        <f t="shared" si="1"/>
+        <v>0.34470000000000001</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="1"/>
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2">
+        <f>LOG(E20)</f>
+        <v>0.62280442780503209</v>
+      </c>
+      <c r="C20" s="2">
+        <f>LOG(F20)</f>
+        <v>0.63972548467876489</v>
+      </c>
+      <c r="E20" s="2">
+        <v>4.1956999999999995</v>
+      </c>
+      <c r="F20" s="2">
+        <v>4.3624000000000001</v>
+      </c>
+      <c r="G20" s="3">
+        <f>1 - (E20/F20)</f>
+        <v>3.8212910324592064E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2">
+        <f t="shared" ref="B21:B26" si="2">LOG(E21)</f>
+        <v>0.71252343487769476</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" ref="C21:C26" si="3">LOG(F21)</f>
+        <v>0.71754568780327022</v>
+      </c>
+      <c r="E21" s="2">
+        <v>5.1585000000000001</v>
+      </c>
+      <c r="F21" s="2">
+        <v>5.2184999999999997</v>
+      </c>
+      <c r="G21" s="3">
+        <f t="shared" ref="G21:G26" si="4">1 - (E21/F21)</f>
+        <v>1.1497556769186512E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2">
+        <f t="shared" si="2"/>
+        <v>2.5991000910235207</v>
+      </c>
+      <c r="C22" s="2">
+        <f t="shared" si="3"/>
+        <v>2.6339489435757018</v>
+      </c>
+      <c r="E22" s="2">
+        <v>397.28309999999999</v>
+      </c>
+      <c r="F22" s="2">
+        <v>430.476</v>
+      </c>
+      <c r="G22" s="3">
+        <f t="shared" si="4"/>
+        <v>7.7107434560811816E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2">
+        <f t="shared" si="2"/>
+        <v>2.0806153047770688</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" si="3"/>
+        <v>2.101603086956763</v>
+      </c>
+      <c r="E23" s="2">
+        <v>120.39689999999999</v>
+      </c>
+      <c r="F23" s="2">
+        <v>126.35810000000001</v>
+      </c>
+      <c r="G23" s="3">
+        <f t="shared" si="4"/>
+        <v>4.7177030993660218E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2">
+        <f t="shared" si="2"/>
+        <v>1.9965449434408036</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" si="3"/>
+        <v>2.0040077945839494</v>
+      </c>
+      <c r="E24" s="2">
+        <v>99.207599999999999</v>
+      </c>
+      <c r="F24" s="2">
+        <v>100.92710000000001</v>
+      </c>
+      <c r="G24" s="3">
+        <f t="shared" si="4"/>
+        <v>1.7037049513956237E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2">
+        <f t="shared" si="2"/>
+        <v>-8.7087448823903096E-2</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" si="3"/>
+        <v>-7.4223946163253715E-2</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.81829999999999992</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.84289999999999998</v>
+      </c>
+      <c r="G25" s="3">
+        <f t="shared" si="4"/>
+        <v>2.9184956697117181E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.46029676105217449</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="3"/>
+        <v>-0.46255871659205239</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.34649999999999997</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.34470000000000001</v>
+      </c>
+      <c r="G26" s="3">
+        <f t="shared" si="4"/>
+        <v>-5.2219321148823106E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>